<commit_message>
finished all website scraping
</commit_message>
<xml_diff>
--- a/Road_Map.xlsx
+++ b/Road_Map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Sam/Desktop/Epson_WS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B878A3-E8AB-DE47-B5FB-E652BB864CA2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941A4F59-B5BC-3741-9086-54379ADDDBA2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4940" yWindow="1020" windowWidth="28040" windowHeight="17440" xr2:uid="{A27A5D58-989B-E34F-8F65-B59C7EA9A8F3}"/>
+    <workbookView xWindow="16420" yWindow="1660" windowWidth="28040" windowHeight="17440" xr2:uid="{A27A5D58-989B-E34F-8F65-B59C7EA9A8F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t>Websites</t>
   </si>
@@ -151,6 +151,12 @@
   </si>
   <si>
     <t>Tiger Direct</t>
+  </si>
+  <si>
+    <t>PC Connection</t>
+  </si>
+  <si>
+    <t>Amazon</t>
   </si>
 </sst>
 </file>
@@ -515,7 +521,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -640,23 +646,40 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
       <c r="B14" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
       <c r="B15" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
       <c r="B16" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>42</v>
+      </c>
       <c r="B17" s="1" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>